<commit_message>
chore: update test cases spreadsheet with latest data
</commit_message>
<xml_diff>
--- a/Test Cases.xlsx
+++ b/Test Cases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SLIIT\Y3S2\Assinment 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20E5BB5B-4402-462C-8ABE-388584FD051B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EA791DB-103E-4073-848E-0B93AE598310}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{14655C8C-63A7-4A34-8F4F-718C9EB73A5A}"/>
   </bookViews>
@@ -540,11 +540,6 @@
     <t>Line Breaks and Paragraph</t>
   </si>
   <si>
-    <t>mama gedara yanavaa
-amma inne
-thaththa awe naha</t>
-  </si>
-  <si>
     <t>මම ගෙදර යනවා
 අම්ම ඉන්නේ
 තත්තා ආවේ නැහැ</t>
@@ -775,44 +770,49 @@
     <t>මෙක rupees 500 යි</t>
   </si>
   <si>
-    <t>මම ගෙඩර යනවා_x000D_
+    <t>මම     ගෙඩර     යනවා</t>
+  </si>
+  <si>
+    <t>ඔයාගෙ email එක සමන්123@gmail.com නේද</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ඔයාගෙ phone එකේ password එක "සඩරුwඅන්345" </t>
+  </si>
+  <si>
+    <t>ඔයාට හ්ට්ට්ප්ස්://www.youtube.com/ මෙ URL එක click කරල youtube එකට යන්න පුලුwඅන්.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">අපි පෙට්ටනෙයට යනwඅ සෙල්ලම් කරන්න. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">මම කම එකක් ගෙනwඅ අපි එක කමු </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ඉක්මනට ඔක ඉwඅර කරල පන්ටියට එන්න </t>
+  </si>
+  <si>
+    <t xml:space="preserve">එක හරිම් කෙතේ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">මම පොලෙcඑ ය්නw </t>
+  </si>
+  <si>
+    <t xml:space="preserve">හරිම පන්ඩෙතෛ ඔය </t>
+  </si>
+  <si>
+    <t>ඇපල් juice එක්ඛ් බොමුඩ්</t>
+  </si>
+  <si>
+    <t>මම ගෙඩර යනවා
+අම්ම ඉන්නේ
+තත්ත awe naha</t>
+  </si>
+  <si>
+    <t>mama gedara yanavaa_x000D_
 _x000D_
-අම්ම ඉන්නේ_x000D_
+amma inne_x000D_
 _x000D_
-තත්ත awe naha</t>
-  </si>
-  <si>
-    <t>මම     ගෙඩර     යනවා</t>
-  </si>
-  <si>
-    <t>ඔයාගෙ email එක සමන්123@gmail.com නේද</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ඔයාගෙ phone එකේ password එක "සඩරුwඅන්345" </t>
-  </si>
-  <si>
-    <t>ඔයාට හ්ට්ට්ප්ස්://www.youtube.com/ මෙ URL එක click කරල youtube එකට යන්න පුලුwඅන්.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">අපි පෙට්ටනෙයට යනwඅ සෙල්ලම් කරන්න. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">මම කම එකක් ගෙනwඅ අපි එක කමු </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ඉක්මනට ඔක ඉwඅර කරල පන්ටියට එන්න </t>
-  </si>
-  <si>
-    <t xml:space="preserve">එක හරිම් කෙතේ </t>
-  </si>
-  <si>
-    <t xml:space="preserve">මම පොලෙcඑ ය්නw </t>
-  </si>
-  <si>
-    <t xml:space="preserve">හරිම පන්ඩෙතෛ ඔය </t>
-  </si>
-  <si>
-    <t>ඇපල් juice එක්ඛ් බොමුඩ්</t>
+thaththa awe naha</t>
   </si>
 </sst>
 </file>
@@ -878,9 +878,6 @@
   </cellStyles>
   <dxfs count="10">
     <dxf>
-      <font>
-        <b/>
-      </font>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
@@ -908,6 +905,9 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
+      <font>
+        <b/>
+      </font>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
   </dxfs>
@@ -945,18 +945,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3EA8A591-FC78-4555-99A1-B3EE67B088D7}" name="test_cases" displayName="test_cases" ref="A1:I41" tableType="queryTable" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3EA8A591-FC78-4555-99A1-B3EE67B088D7}" name="test_cases" displayName="test_cases" ref="A1:I41" tableType="queryTable" totalsRowShown="0" headerRowDxfId="9">
   <autoFilter ref="A1:I41" xr:uid="{3EA8A591-FC78-4555-99A1-B3EE67B088D7}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{192B81A1-AE56-470C-809A-881EE2728319}" uniqueName="1" name="TC ID" queryTableFieldId="1" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{F75C041F-AF3B-4988-9FF5-4012D96932F9}" uniqueName="2" name="Test Case Name" queryTableFieldId="2" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{35AD8064-5DB6-4FA7-8770-29513A6E757B}" uniqueName="3" name="Input Length Type" queryTableFieldId="3" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{2A36C8E3-AE5A-498C-886C-9D664837D249}" uniqueName="4" name="Input (Singlish)" queryTableFieldId="4" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{7F21281E-5758-42B4-8B98-6653D5E6A031}" uniqueName="5" name="Expected Output (Sinhala)" queryTableFieldId="5" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{DFE13DF3-DE9D-4B16-9D70-C3D5DA0C6755}" uniqueName="6" name="Actual Output" queryTableFieldId="6" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{E6C1545C-6DFF-4612-9E45-922CBEF43A59}" uniqueName="7" name="Status" queryTableFieldId="7" dataDxfId="3"/>
-    <tableColumn id="9" xr3:uid="{0F460C68-2CD5-4FF9-B4A5-E77237C63305}" uniqueName="9" name="Accuracy Justification / Issue Description" queryTableFieldId="9" dataDxfId="2"/>
-    <tableColumn id="10" xr3:uid="{79924D07-C61F-4C8C-8BBE-2B74BFF30390}" uniqueName="10" name="What is covered by the test" queryTableFieldId="10" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{192B81A1-AE56-470C-809A-881EE2728319}" uniqueName="1" name="TC ID" queryTableFieldId="1" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{F75C041F-AF3B-4988-9FF5-4012D96932F9}" uniqueName="2" name="Test Case Name" queryTableFieldId="2" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{35AD8064-5DB6-4FA7-8770-29513A6E757B}" uniqueName="3" name="Input Length Type" queryTableFieldId="3" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{2A36C8E3-AE5A-498C-886C-9D664837D249}" uniqueName="4" name="Input (Singlish)" queryTableFieldId="4" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{7F21281E-5758-42B4-8B98-6653D5E6A031}" uniqueName="5" name="Expected Output (Sinhala)" queryTableFieldId="5" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{DFE13DF3-DE9D-4B16-9D70-C3D5DA0C6755}" uniqueName="6" name="Actual Output" queryTableFieldId="6" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{E6C1545C-6DFF-4612-9E45-922CBEF43A59}" uniqueName="7" name="Status" queryTableFieldId="7" dataDxfId="2"/>
+    <tableColumn id="9" xr3:uid="{0F460C68-2CD5-4FF9-B4A5-E77237C63305}" uniqueName="9" name="Accuracy Justification / Issue Description" queryTableFieldId="9" dataDxfId="1"/>
+    <tableColumn id="10" xr3:uid="{79924D07-C61F-4C8C-8BBE-2B74BFF30390}" uniqueName="10" name="What is covered by the test" queryTableFieldId="10" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1261,8 +1261,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3F027FF-56AC-4236-BE94-07887FD85E21}">
   <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="G2" zoomScale="84" zoomScaleNormal="22" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1962,7 +1962,7 @@
         <v>140</v>
       </c>
       <c r="F24" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="G24" t="s">
         <v>141</v>
@@ -2049,7 +2049,7 @@
         <v>159</v>
       </c>
       <c r="F27" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="G27" t="s">
         <v>141</v>
@@ -2061,7 +2061,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" ht="72" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>162</v>
       </c>
@@ -2071,78 +2071,78 @@
       <c r="C28" t="s">
         <v>19</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D28" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="E28" t="s">
         <v>164</v>
       </c>
-      <c r="E28" t="s">
-        <v>165</v>
-      </c>
       <c r="F28" s="2" t="s">
-        <v>241</v>
+        <v>251</v>
       </c>
       <c r="G28" t="s">
         <v>141</v>
       </c>
       <c r="H28" t="s">
+        <v>165</v>
+      </c>
+      <c r="I28" t="s">
         <v>166</v>
-      </c>
-      <c r="I28" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
+        <v>167</v>
+      </c>
+      <c r="B29" t="s">
         <v>168</v>
       </c>
-      <c r="B29" t="s">
+      <c r="C29" t="s">
         <v>169</v>
       </c>
-      <c r="C29" t="s">
+      <c r="D29" t="s">
         <v>170</v>
       </c>
-      <c r="D29" t="s">
+      <c r="E29" t="s">
+        <v>237</v>
+      </c>
+      <c r="F29" t="s">
+        <v>237</v>
+      </c>
+      <c r="G29" t="s">
+        <v>14</v>
+      </c>
+      <c r="H29" t="s">
         <v>171</v>
       </c>
-      <c r="E29" t="s">
-        <v>238</v>
-      </c>
-      <c r="F29" t="s">
-        <v>238</v>
-      </c>
-      <c r="G29" t="s">
-        <v>14</v>
-      </c>
-      <c r="H29" t="s">
+      <c r="I29" t="s">
         <v>172</v>
-      </c>
-      <c r="I29" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
+        <v>173</v>
+      </c>
+      <c r="B30" t="s">
         <v>174</v>
       </c>
-      <c r="B30" t="s">
+      <c r="C30" t="s">
+        <v>19</v>
+      </c>
+      <c r="D30" t="s">
         <v>175</v>
       </c>
-      <c r="C30" t="s">
-        <v>19</v>
-      </c>
-      <c r="D30" t="s">
+      <c r="E30" t="s">
         <v>176</v>
       </c>
-      <c r="E30" t="s">
+      <c r="F30" t="s">
+        <v>176</v>
+      </c>
+      <c r="G30" t="s">
+        <v>14</v>
+      </c>
+      <c r="H30" t="s">
         <v>177</v>
-      </c>
-      <c r="F30" t="s">
-        <v>177</v>
-      </c>
-      <c r="G30" t="s">
-        <v>14</v>
-      </c>
-      <c r="H30" t="s">
-        <v>178</v>
       </c>
       <c r="I30" t="s">
         <v>136</v>
@@ -2150,321 +2150,321 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
+        <v>178</v>
+      </c>
+      <c r="B31" t="s">
         <v>179</v>
       </c>
-      <c r="B31" t="s">
+      <c r="C31" t="s">
+        <v>19</v>
+      </c>
+      <c r="D31" t="s">
         <v>180</v>
       </c>
-      <c r="C31" t="s">
-        <v>19</v>
-      </c>
-      <c r="D31" t="s">
+      <c r="E31" t="s">
         <v>181</v>
       </c>
-      <c r="E31" t="s">
+      <c r="F31" t="s">
+        <v>181</v>
+      </c>
+      <c r="G31" t="s">
+        <v>14</v>
+      </c>
+      <c r="H31" t="s">
         <v>182</v>
       </c>
-      <c r="F31" t="s">
-        <v>182</v>
-      </c>
-      <c r="G31" t="s">
-        <v>14</v>
-      </c>
-      <c r="H31" t="s">
+      <c r="I31" t="s">
         <v>183</v>
-      </c>
-      <c r="I31" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
+        <v>184</v>
+      </c>
+      <c r="B32" t="s">
         <v>185</v>
       </c>
-      <c r="B32" t="s">
+      <c r="C32" t="s">
+        <v>19</v>
+      </c>
+      <c r="D32" t="s">
         <v>186</v>
       </c>
-      <c r="C32" t="s">
-        <v>19</v>
-      </c>
-      <c r="D32" t="s">
+      <c r="E32" t="s">
         <v>187</v>
       </c>
-      <c r="E32" t="s">
-        <v>188</v>
-      </c>
       <c r="F32" s="3" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="G32" t="s">
         <v>141</v>
       </c>
       <c r="H32" t="s">
+        <v>188</v>
+      </c>
+      <c r="I32" t="s">
         <v>189</v>
-      </c>
-      <c r="I32" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
+        <v>190</v>
+      </c>
+      <c r="B33" t="s">
         <v>191</v>
       </c>
-      <c r="B33" t="s">
+      <c r="C33" t="s">
+        <v>19</v>
+      </c>
+      <c r="D33" t="s">
         <v>192</v>
       </c>
-      <c r="C33" t="s">
-        <v>19</v>
-      </c>
-      <c r="D33" t="s">
+      <c r="E33" t="s">
         <v>193</v>
       </c>
-      <c r="E33" t="s">
-        <v>194</v>
-      </c>
       <c r="F33" s="3" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G33" t="s">
         <v>141</v>
       </c>
       <c r="H33" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="I33" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="34" spans="1:9" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
+        <v>195</v>
+      </c>
+      <c r="B34" t="s">
         <v>196</v>
       </c>
-      <c r="B34" t="s">
+      <c r="C34" t="s">
+        <v>19</v>
+      </c>
+      <c r="D34" t="s">
         <v>197</v>
       </c>
-      <c r="C34" t="s">
-        <v>19</v>
-      </c>
-      <c r="D34" t="s">
+      <c r="E34" t="s">
         <v>198</v>
       </c>
-      <c r="E34" t="s">
-        <v>199</v>
-      </c>
       <c r="F34" s="3" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="G34" t="s">
         <v>141</v>
       </c>
       <c r="H34" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="I34" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="35" spans="1:9" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
+        <v>200</v>
+      </c>
+      <c r="B35" t="s">
         <v>201</v>
       </c>
-      <c r="B35" t="s">
+      <c r="C35" t="s">
+        <v>19</v>
+      </c>
+      <c r="D35" t="s">
         <v>202</v>
       </c>
-      <c r="C35" t="s">
-        <v>19</v>
-      </c>
-      <c r="D35" t="s">
+      <c r="E35" t="s">
         <v>203</v>
       </c>
-      <c r="E35" t="s">
-        <v>204</v>
-      </c>
       <c r="F35" s="3" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="G35" t="s">
         <v>141</v>
       </c>
       <c r="H35" t="s">
+        <v>204</v>
+      </c>
+      <c r="I35" t="s">
         <v>205</v>
-      </c>
-      <c r="I35" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="36" spans="1:9" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
+        <v>206</v>
+      </c>
+      <c r="B36" t="s">
         <v>207</v>
       </c>
-      <c r="B36" t="s">
+      <c r="C36" t="s">
+        <v>19</v>
+      </c>
+      <c r="D36" t="s">
         <v>208</v>
       </c>
-      <c r="C36" t="s">
-        <v>19</v>
-      </c>
-      <c r="D36" t="s">
+      <c r="E36" t="s">
         <v>209</v>
       </c>
-      <c r="E36" t="s">
-        <v>210</v>
-      </c>
       <c r="F36" s="3" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="G36" t="s">
         <v>141</v>
       </c>
       <c r="H36" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I36" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="37" spans="1:9" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
+        <v>211</v>
+      </c>
+      <c r="B37" t="s">
         <v>212</v>
       </c>
-      <c r="B37" t="s">
+      <c r="C37" t="s">
+        <v>19</v>
+      </c>
+      <c r="D37" t="s">
         <v>213</v>
       </c>
-      <c r="C37" t="s">
-        <v>19</v>
-      </c>
-      <c r="D37" t="s">
+      <c r="E37" t="s">
         <v>214</v>
       </c>
-      <c r="E37" t="s">
-        <v>215</v>
-      </c>
       <c r="F37" s="3" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="G37" t="s">
         <v>141</v>
       </c>
       <c r="H37" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="I37" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="38" spans="1:9" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
+        <v>216</v>
+      </c>
+      <c r="B38" t="s">
         <v>217</v>
       </c>
-      <c r="B38" t="s">
+      <c r="C38" t="s">
+        <v>19</v>
+      </c>
+      <c r="D38" t="s">
         <v>218</v>
       </c>
-      <c r="C38" t="s">
-        <v>19</v>
-      </c>
-      <c r="D38" t="s">
+      <c r="E38" t="s">
         <v>219</v>
       </c>
-      <c r="E38" t="s">
-        <v>220</v>
-      </c>
       <c r="F38" s="3" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="G38" t="s">
         <v>141</v>
       </c>
       <c r="H38" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="I38" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="39" spans="1:9" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
+        <v>221</v>
+      </c>
+      <c r="B39" t="s">
         <v>222</v>
       </c>
-      <c r="B39" t="s">
+      <c r="C39" t="s">
+        <v>19</v>
+      </c>
+      <c r="D39" t="s">
         <v>223</v>
       </c>
-      <c r="C39" t="s">
-        <v>19</v>
-      </c>
-      <c r="D39" t="s">
+      <c r="E39" t="s">
         <v>224</v>
       </c>
-      <c r="E39" t="s">
-        <v>225</v>
-      </c>
       <c r="F39" s="3" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="G39" t="s">
         <v>141</v>
       </c>
       <c r="H39" t="s">
+        <v>225</v>
+      </c>
+      <c r="I39" t="s">
         <v>226</v>
-      </c>
-      <c r="I39" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="40" spans="1:9" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
+        <v>227</v>
+      </c>
+      <c r="B40" t="s">
         <v>228</v>
       </c>
-      <c r="B40" t="s">
+      <c r="C40" t="s">
+        <v>19</v>
+      </c>
+      <c r="D40" t="s">
         <v>229</v>
       </c>
-      <c r="C40" t="s">
-        <v>19</v>
-      </c>
-      <c r="D40" t="s">
+      <c r="E40" t="s">
         <v>230</v>
       </c>
-      <c r="E40" t="s">
-        <v>231</v>
-      </c>
       <c r="F40" s="3" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="G40" t="s">
         <v>141</v>
       </c>
       <c r="H40" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="I40" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="41" spans="1:9" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
+        <v>232</v>
+      </c>
+      <c r="B41" t="s">
         <v>233</v>
       </c>
-      <c r="B41" t="s">
+      <c r="C41" t="s">
+        <v>19</v>
+      </c>
+      <c r="D41" t="s">
+        <v>238</v>
+      </c>
+      <c r="E41" t="s">
         <v>234</v>
       </c>
-      <c r="C41" t="s">
-        <v>19</v>
-      </c>
-      <c r="D41" t="s">
-        <v>239</v>
-      </c>
-      <c r="E41" t="s">
-        <v>235</v>
-      </c>
       <c r="F41" s="4" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="G41" t="s">
         <v>141</v>
       </c>
       <c r="H41" t="s">
+        <v>235</v>
+      </c>
+      <c r="I41" t="s">
         <v>236</v>
-      </c>
-      <c r="I41" t="s">
-        <v>237</v>
       </c>
     </row>
   </sheetData>

</xml_diff>